<commit_message>
update Task VS 41b7d460d23872a4a9cca8748cff9529ccca42b8
</commit_message>
<xml_diff>
--- a/393-contenu-fhir---gestion-des-slices-remontant-un-warning/ig/StructureDefinition-tddui-task-action.xlsx
+++ b/393-contenu-fhir---gestion-des-slices-remontant-un-warning/ig/StructureDefinition-tddui-task-action.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4368" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4361" uniqueCount="627">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-17T09:55:45+00:00</t>
+    <t>2025-12-17T14:41:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1702,7 +1702,7 @@
     <t>Inputs are named to enable task automation to bind data and pass it from one task to the next.</t>
   </si>
   <si>
-    <t>Codes to identify types of input parameters.  These will typically be specific to a particular workflow.  E.g. "Comparison source", "Applicable consent", "Concomitent Medications", etc.</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/tddui/ValueSet/input-tddui-task-action-valueset</t>
   </si>
   <si>
     <t>Task.input.value[x]</t>
@@ -2320,8 +2320,8 @@
     <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="145.00390625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="39.265625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="143.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="67.0390625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
@@ -10936,13 +10936,11 @@
         <v>78</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Y74" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y74" s="2"/>
+      <c r="Z74" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AA74" t="s" s="2">
         <v>78</v>
@@ -11640,13 +11638,11 @@
         <v>78</v>
       </c>
       <c r="X80" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Y80" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y80" s="2"/>
+      <c r="Z80" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="Z80" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AA80" t="s" s="2">
         <v>78</v>
@@ -12344,13 +12340,11 @@
         <v>78</v>
       </c>
       <c r="X86" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Y86" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y86" s="2"/>
+      <c r="Z86" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="Z86" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AA86" t="s" s="2">
         <v>78</v>
@@ -13048,13 +13042,11 @@
         <v>78</v>
       </c>
       <c r="X92" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Y92" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y92" s="2"/>
+      <c r="Z92" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="Z92" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AA92" t="s" s="2">
         <v>78</v>
@@ -13752,13 +13744,11 @@
         <v>78</v>
       </c>
       <c r="X98" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Y98" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y98" s="2"/>
+      <c r="Z98" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="Z98" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AA98" t="s" s="2">
         <v>78</v>
@@ -14456,13 +14446,11 @@
         <v>78</v>
       </c>
       <c r="X104" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Y104" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y104" s="2"/>
+      <c r="Z104" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="Z104" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AA104" t="s" s="2">
         <v>78</v>
@@ -15160,13 +15148,11 @@
         <v>78</v>
       </c>
       <c r="X110" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="Y110" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="Y110" s="2"/>
+      <c r="Z110" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="Z110" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="AA110" t="s" s="2">
         <v>78</v>

</xml_diff>